<commit_message>
Updated template with numbers for categories
</commit_message>
<xml_diff>
--- a/docs/sheets/GreenIT_Template_1.xlsx
+++ b/docs/sheets/GreenIT_Template_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l_you\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1836336-4568-485B-AFB0-6F1C04A6BF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E508D5E-3F19-4B97-8F84-695F88E602C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1399AF25-A898-4F96-B3AC-1A8623F40788}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>isSupportingFactor</t>
   </si>
   <si>
-    <t>De groene interventie</t>
-  </si>
-  <si>
     <t>#FF0000</t>
   </si>
   <si>
@@ -266,9 +263,6 @@
     <t>Er zijn duidelijke afspraken over wie verantwoordelijk is voor het onderhoud en beheer van het groen</t>
   </si>
   <si>
-    <t>De externe omgeving</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kenmerken van de externe omgeving die van invloed zijn op de implementatie </t>
   </si>
   <si>
@@ -302,9 +296,6 @@
     <t>Vanuit externe centrale instanties zoals de overheid, brancheverenigingen en zorgverzekeraars wordt bijvoorbeeld via beleid, richtlijnen, subsidies en aanbevelingen implementatie van groene interventies binnen zorginstellingen ondersteund</t>
   </si>
   <si>
-    <t>De organisatie</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kenmerken van de organisatie die van invloed zijn op de implementatie </t>
   </si>
   <si>
@@ -416,9 +407,6 @@
     <t xml:space="preserve">Er is scholing en trainingen waarin betrokkenen leren hoe ze de groene interventie kunnen gebruiken en onderhouden  </t>
   </si>
   <si>
-    <t>Kenmerken betrokkenen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kenmerken van betrokkenen die van invloed zijn op de implementatie </t>
   </si>
   <si>
@@ -452,9 +440,6 @@
     <t>Betrokkenen bezitten persoonlijke eigenschappen die een positieve invloed kunnen hebben op de implementatie, zoals intellectuele competentie, motivatie, waarden, vaardigheden, capaciteit, innovativiteit, passie, energie, doorzettingsvermogen, geduld, vermogen om kansen te grijpen, ervaring en leergierigheid</t>
   </si>
   <si>
-    <t>Proces</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kenmerken van het proces die van invloed zijn op de implementatie </t>
   </si>
   <si>
@@ -552,6 +537,21 @@
   </si>
   <si>
     <t>Medewerkers beschouwen het gebruik van de groene interventie als onderdeel van hun werk in plaats van als afleiding van hun 'echte' werk</t>
+  </si>
+  <si>
+    <t>1. De groene interventie</t>
+  </si>
+  <si>
+    <t>2. De externe omgeving</t>
+  </si>
+  <si>
+    <t>3. De organisatie</t>
+  </si>
+  <si>
+    <t>4. Kenmerken betrokkenen</t>
+  </si>
+  <si>
+    <t>5. Proces</t>
   </si>
 </sst>
 </file>
@@ -666,6 +666,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -673,9 +676,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B554B7-16E3-4364-AB12-1AF0F5EB24FC}">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1032,20 +1032,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1074,39 +1074,39 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G4" s="1">
         <v>2</v>
@@ -1116,17 +1116,17 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="9">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G5" s="1">
         <v>3</v>
@@ -1136,13 +1136,13 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1">
         <v>4</v>
@@ -1152,17 +1152,17 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1">
         <v>5</v>
@@ -1172,17 +1172,17 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1">
         <v>6</v>
@@ -1192,17 +1192,17 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1">
         <v>7</v>
@@ -1212,17 +1212,17 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E10" s="9">
-        <v>6</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="G10" s="1">
         <v>8</v>
@@ -1232,13 +1232,13 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1">
         <v>9</v>
@@ -1248,17 +1248,17 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="6">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E12" s="9">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="G12" s="1">
         <v>10</v>
@@ -1268,13 +1268,13 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="1">
         <v>11</v>
@@ -1284,17 +1284,17 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="6">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E14" s="9">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G14" s="1">
         <v>12</v>
@@ -1304,13 +1304,13 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="1">
         <v>13</v>
@@ -1320,17 +1320,17 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="6">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E16" s="9">
-        <v>9</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G16" s="1">
         <v>14</v>
@@ -1340,13 +1340,13 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" s="1">
         <v>15</v>
@@ -1356,17 +1356,17 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="6">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E18" s="9">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="G18" s="1">
         <v>16</v>
@@ -1376,13 +1376,13 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="1">
         <v>17</v>
@@ -1392,13 +1392,13 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="1">
         <v>18</v>
@@ -1408,13 +1408,13 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
       <c r="F21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" s="1">
         <v>19</v>
@@ -1424,13 +1424,13 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
       <c r="F22" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G22" s="1">
         <v>20</v>
@@ -1440,13 +1440,13 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
       <c r="F23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G23" s="1">
         <v>21</v>
@@ -1456,17 +1456,17 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="6">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E24" s="9">
-        <v>11</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="G24" s="1">
         <v>22</v>
@@ -1476,13 +1476,13 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
       <c r="F25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G25" s="1">
         <v>23</v>
@@ -1492,17 +1492,17 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" s="1">
         <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G26" s="1">
         <v>24</v>
@@ -1512,17 +1512,17 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9" t="s">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="6">
+        <v>13</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E27" s="9">
-        <v>13</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="G27" s="1">
         <v>25</v>
@@ -1532,13 +1532,13 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G28" s="1">
         <v>26</v>
@@ -1548,13 +1548,13 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G29" s="1">
         <v>27</v>
@@ -1564,13 +1564,13 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
       <c r="F30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G30" s="1">
         <v>28</v>
@@ -1580,17 +1580,17 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E31" s="1">
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G31" s="1">
         <v>29</v>
@@ -1600,17 +1600,17 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="1">
         <v>15</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G32" s="1">
         <v>30</v>
@@ -1620,17 +1620,17 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E33" s="1">
         <v>16</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G33" s="1">
         <v>31</v>
@@ -1640,17 +1640,17 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9" t="s">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="6">
+        <v>17</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E34" s="9">
-        <v>17</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G34" s="1">
         <v>32</v>
@@ -1660,13 +1660,13 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
       <c r="F35" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G35" s="1">
         <v>33</v>
@@ -1676,13 +1676,13 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
       <c r="F36" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G36" s="1">
         <v>34</v>
@@ -1692,13 +1692,13 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
       <c r="F37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" s="1">
         <v>35</v>
@@ -1708,13 +1708,13 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
       <c r="F38" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G38" s="1">
         <v>36</v>
@@ -1724,13 +1724,13 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
       <c r="F39" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G39" s="1">
         <v>37</v>
@@ -1740,17 +1740,17 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="9">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="6">
         <v>18</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G40" s="1">
         <v>38</v>
@@ -1760,13 +1760,13 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
       <c r="F41" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G41" s="1">
         <v>39</v>
@@ -1776,13 +1776,13 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
       <c r="F42" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G42" s="1">
         <v>40</v>
@@ -1792,13 +1792,13 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
       <c r="F43" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G43" s="1">
         <v>41</v>
@@ -1808,13 +1808,13 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
       <c r="F44" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G44" s="1">
         <v>42</v>
@@ -1824,13 +1824,13 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
       <c r="F45" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G45" s="1">
         <v>43</v>
@@ -1840,13 +1840,13 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
       <c r="F46" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G46" s="1">
         <v>44</v>
@@ -1856,13 +1856,13 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
       <c r="F47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G47" s="1">
         <v>45</v>
@@ -1872,17 +1872,17 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="6">
+        <v>19</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E48" s="9">
-        <v>19</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="G48" s="1">
         <v>46</v>
@@ -1892,13 +1892,13 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G49" s="1">
         <v>47</v>
@@ -1908,23 +1908,23 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" s="9" t="s">
+      <c r="E50" s="6">
+        <v>20</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E50" s="9">
-        <v>20</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="G50" s="1">
         <v>48</v>
@@ -1934,13 +1934,13 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
       <c r="F51" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G51" s="1">
         <v>49</v>
@@ -1950,13 +1950,13 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
       <c r="F52" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G52" s="1">
         <v>50</v>
@@ -1966,17 +1966,17 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E53" s="9">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53" s="6">
         <v>21</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G53" s="1">
         <v>51</v>
@@ -1986,13 +1986,13 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
       <c r="F54" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G54" s="1">
         <v>52</v>
@@ -2002,17 +2002,17 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E55" s="9">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" s="6">
         <v>22</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G55" s="1">
         <v>53</v>
@@ -2022,13 +2022,13 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
       <c r="F56" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G56" s="1">
         <v>54</v>
@@ -2038,23 +2038,23 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>89</v>
+      <c r="A57" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E57" s="1">
         <v>23</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G57" s="1">
         <v>55</v>
@@ -2064,17 +2064,17 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
       <c r="D58" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E58" s="1">
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G58" s="1">
         <v>56</v>
@@ -2084,17 +2084,17 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
       <c r="D59" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E59" s="1">
         <v>25</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G59" s="1">
         <v>57</v>
@@ -2104,17 +2104,17 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
       <c r="D60" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E60" s="1">
         <v>26</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G60" s="1">
         <v>58</v>
@@ -2124,17 +2124,17 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="9"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E61" s="9">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E61" s="6">
         <v>27</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G61" s="1">
         <v>59</v>
@@ -2144,13 +2144,13 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
-      <c r="B62" s="9"/>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
       <c r="F62" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G62" s="1">
         <v>60</v>
@@ -2160,17 +2160,17 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E63" s="9">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" s="6">
         <v>28</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G63" s="1">
         <v>61</v>
@@ -2180,13 +2180,13 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="9"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
       <c r="F64" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G64" s="1">
         <v>62</v>
@@ -2196,13 +2196,13 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
       <c r="F65" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G65" s="1">
         <v>63</v>
@@ -2212,17 +2212,17 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
       <c r="D66" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E66" s="1">
         <v>29</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G66" s="1">
         <v>64</v>
@@ -2232,17 +2232,17 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E67" s="9">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E67" s="6">
         <v>30</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G67" s="1">
         <v>65</v>
@@ -2252,13 +2252,13 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
       <c r="F68" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G68" s="1">
         <v>66</v>
@@ -2268,13 +2268,13 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
       <c r="F69" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G69" s="1">
         <v>67</v>
@@ -2284,13 +2284,13 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="9"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="9"/>
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
       <c r="F70" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G70" s="1">
         <v>68</v>
@@ -2300,17 +2300,17 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
       <c r="D71" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E71" s="1">
         <v>31</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G71" s="1">
         <v>69</v>
@@ -2320,17 +2320,17 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
       <c r="D72" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E72" s="1">
         <v>32</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G72" s="1">
         <v>70</v>
@@ -2340,17 +2340,17 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E73" s="9">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E73" s="6">
         <v>33</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G73" s="1">
         <v>71</v>
@@ -2360,13 +2360,13 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
+      <c r="A74" s="6"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
       <c r="F74" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G74" s="1">
         <v>72</v>
@@ -2376,13 +2376,13 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="9"/>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
       <c r="F75" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G75" s="1">
         <v>73</v>
@@ -2392,13 +2392,13 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
       <c r="F76" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G76" s="1">
         <v>74</v>
@@ -2408,13 +2408,13 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
       <c r="F77" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G77" s="1">
         <v>75</v>
@@ -2424,13 +2424,13 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="9"/>
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
       <c r="F78" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G78" s="1">
         <v>76</v>
@@ -2440,13 +2440,13 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="9"/>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
       <c r="F79" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G79" s="1">
         <v>77</v>
@@ -2456,17 +2456,17 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="9"/>
-      <c r="B80" s="9"/>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E80" s="9">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E80" s="6">
         <v>34</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G80" s="1">
         <v>78</v>
@@ -2476,13 +2476,13 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
-      <c r="E81" s="9"/>
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
       <c r="F81" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G81" s="1">
         <v>79</v>
@@ -2492,23 +2492,23 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>127</v>
+      <c r="A82" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E82" s="1">
         <v>35</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G82" s="1">
         <v>80</v>
@@ -2518,17 +2518,17 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
       <c r="D83" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E83" s="1">
         <v>36</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G83" s="1">
         <v>81</v>
@@ -2538,17 +2538,17 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="9"/>
-      <c r="B84" s="9"/>
-      <c r="C84" s="9"/>
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
       <c r="D84" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E84" s="1">
         <v>37</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G84" s="1">
         <v>82</v>
@@ -2558,17 +2558,17 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
       <c r="D85" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E85" s="1">
         <v>38</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G85" s="1">
         <v>83</v>
@@ -2578,17 +2578,17 @@
       </c>
     </row>
     <row r="86" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
       <c r="D86" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E86" s="1">
         <v>39</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G86" s="1">
         <v>84</v>
@@ -2598,23 +2598,23 @@
       </c>
     </row>
     <row r="87" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B87" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>139</v>
+      <c r="A87" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>134</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E87" s="1">
         <v>40</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G87" s="1">
         <v>85</v>
@@ -2624,17 +2624,17 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="9"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
+      <c r="A88" s="6"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
       <c r="D88" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E88" s="1">
         <v>41</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G88" s="1">
         <v>86</v>
@@ -2644,17 +2644,17 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="9"/>
-      <c r="B89" s="9"/>
-      <c r="C89" s="9"/>
+      <c r="A89" s="6"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
       <c r="D89" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E89" s="1">
         <v>42</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G89" s="1">
         <v>87</v>
@@ -2664,17 +2664,17 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="9"/>
-      <c r="B90" s="9"/>
-      <c r="C90" s="9"/>
-      <c r="D90" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E90" s="9">
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E90" s="6">
         <v>43</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G90" s="1">
         <v>88</v>
@@ -2684,13 +2684,13 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
+      <c r="A91" s="6"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
       <c r="F91" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G91" s="1">
         <v>89</v>
@@ -2700,13 +2700,13 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="9"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-      <c r="E92" s="9"/>
+      <c r="A92" s="6"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
       <c r="F92" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G92" s="1">
         <v>90</v>
@@ -2716,17 +2716,17 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="9"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E93" s="9">
+      <c r="A93" s="6"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E93" s="6">
         <v>44</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G93" s="1">
         <v>91</v>
@@ -2736,13 +2736,13 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9"/>
-      <c r="E94" s="9"/>
+      <c r="A94" s="6"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
       <c r="F94" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G94" s="1">
         <v>92</v>
@@ -2752,17 +2752,17 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="9"/>
-      <c r="D95" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="E95" s="9">
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E95" s="6">
         <v>45</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G95" s="1">
         <v>93</v>
@@ -2772,13 +2772,13 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="9"/>
-      <c r="E96" s="9"/>
+      <c r="A96" s="6"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
       <c r="F96" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G96" s="1">
         <v>94</v>
@@ -2788,13 +2788,13 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="9"/>
-      <c r="B97" s="9"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="9"/>
-      <c r="E97" s="9"/>
+      <c r="A97" s="6"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
       <c r="F97" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G97" s="1">
         <v>95</v>
@@ -2804,13 +2804,13 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-      <c r="E98" s="9"/>
+      <c r="A98" s="6"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
       <c r="F98" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G98" s="1">
         <v>96</v>
@@ -2820,13 +2820,13 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="9"/>
-      <c r="B99" s="9"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-      <c r="E99" s="9"/>
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
       <c r="F99" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G99" s="1">
         <v>97</v>
@@ -2836,17 +2836,17 @@
       </c>
     </row>
     <row r="100" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
       <c r="D100" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E100" s="1">
         <v>46</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G100" s="1">
         <v>98</v>
@@ -2856,17 +2856,17 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="9"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
+      <c r="A101" s="6"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
       <c r="D101" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E101" s="1">
         <v>47</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G101" s="1">
         <v>99</v>
@@ -2876,17 +2876,17 @@
       </c>
     </row>
     <row r="102" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="9"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="E102" s="9">
+      <c r="A102" s="6"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E102" s="6">
         <v>48</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G102" s="1">
         <v>100</v>
@@ -2896,13 +2896,13 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="9"/>
-      <c r="B103" s="9"/>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9"/>
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
       <c r="F103" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G103" s="1">
         <v>101</v>
@@ -2912,13 +2912,13 @@
       </c>
     </row>
     <row r="104" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="9"/>
-      <c r="B104" s="9"/>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
+      <c r="A104" s="6"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
       <c r="F104" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G104" s="1">
         <v>102</v>
@@ -2928,13 +2928,13 @@
       </c>
     </row>
     <row r="105" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="9"/>
-      <c r="B105" s="9"/>
-      <c r="C105" s="9"/>
-      <c r="D105" s="9"/>
-      <c r="E105" s="9"/>
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
       <c r="F105" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G105" s="1">
         <v>103</v>
@@ -2944,13 +2944,13 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="9"/>
-      <c r="B106" s="9"/>
-      <c r="C106" s="9"/>
-      <c r="D106" s="9"/>
-      <c r="E106" s="9"/>
+      <c r="A106" s="6"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
       <c r="F106" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G106" s="1">
         <v>104</v>
@@ -2961,17 +2961,45 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="E102:E106"/>
-    <mergeCell ref="A87:A106"/>
-    <mergeCell ref="B87:B106"/>
-    <mergeCell ref="C87:C106"/>
-    <mergeCell ref="D90:D92"/>
-    <mergeCell ref="E90:E92"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="D95:D99"/>
-    <mergeCell ref="E95:E99"/>
-    <mergeCell ref="D102:D106"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A3:A49"/>
+    <mergeCell ref="B3:B49"/>
+    <mergeCell ref="C3:C49"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="D34:D39"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="E40:E47"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="B50:B56"/>
+    <mergeCell ref="C50:C56"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="E55:E56"/>
     <mergeCell ref="E73:E79"/>
     <mergeCell ref="D80:D81"/>
     <mergeCell ref="E80:E81"/>
@@ -2988,45 +3016,17 @@
     <mergeCell ref="D67:D70"/>
     <mergeCell ref="E67:E70"/>
     <mergeCell ref="D73:D79"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="B50:B56"/>
-    <mergeCell ref="C50:C56"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="D34:D39"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="E40:E47"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="E18:E23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="A3:A49"/>
-    <mergeCell ref="B3:B49"/>
-    <mergeCell ref="C3:C49"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E102:E106"/>
+    <mergeCell ref="A87:A106"/>
+    <mergeCell ref="B87:B106"/>
+    <mergeCell ref="C87:C106"/>
+    <mergeCell ref="D90:D92"/>
+    <mergeCell ref="E90:E92"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="D95:D99"/>
+    <mergeCell ref="E95:E99"/>
+    <mergeCell ref="D102:D106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>